<commit_message>
updating mya price dataset
</commit_message>
<xml_diff>
--- a/data-raw/fsaArcPlc/input_data/fsaMyaPrice/MYA_2023.xlsx
+++ b/data-raw/fsaArcPlc/input_data/fsaMyaPrice/MYA_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\EPAS\2014FBIMP\ARC_PLC\Webpage Posting\2024-0208\Program Year 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\EPAS\2014FBIMP\ARC_PLC\Webpage Posting\2025-0131\Program Year 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B565BB9-AEA4-45FC-A384-183DA11662DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE85916-3340-4B9A-87CE-61DEC4AAD92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MYA Prices" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <t>TABLE 1. 2017/18-2023/24 MARKET YEAR AVERAGE (MYA) PRICES</t>
   </si>
   <si>
-    <t>February 8, 2024 1/</t>
+    <t>January 31, 2025 1/</t>
   </si>
   <si>
     <t>Commodity</t>
@@ -73,7 +73,7 @@
     <t>Bushel</t>
   </si>
   <si>
-    <t>P</t>
+    <t>F</t>
   </si>
   <si>
     <t>Barley</t>
@@ -188,10 +188,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -204,16 +203,19 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -373,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -410,28 +412,19 @@
     <xf numFmtId="165" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -605,36 +598,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
     </row>
     <row r="4" spans="1:12" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -667,10 +660,10 @@
       <c r="J4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="25"/>
+      <c r="L4" s="22"/>
     </row>
     <row r="5" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -704,7 +697,7 @@
         <v>8.83</v>
       </c>
       <c r="K5" s="6">
-        <v>7.2</v>
+        <v>6.96</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>17</v>
@@ -742,7 +735,7 @@
         <v>7.4</v>
       </c>
       <c r="K6" s="6">
-        <v>7.5</v>
+        <v>7.39</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>17</v>
@@ -780,7 +773,7 @@
         <v>4.57</v>
       </c>
       <c r="K7" s="6">
-        <v>3.7</v>
+        <v>3.92</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>17</v>
@@ -818,7 +811,7 @@
         <v>0.26800000000000002</v>
       </c>
       <c r="K8" s="10">
-        <v>0.27500000000000002</v>
+        <v>0.26900000000000002</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>17</v>
@@ -856,7 +849,7 @@
         <v>6.54</v>
       </c>
       <c r="K9" s="6">
-        <v>4.8</v>
+        <v>4.55</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>17</v>
@@ -894,7 +887,7 @@
         <v>5.94</v>
       </c>
       <c r="K10" s="6">
-        <v>4.8499999999999996</v>
+        <v>4.93</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>17</v>
@@ -932,7 +925,7 @@
         <v>14.2</v>
       </c>
       <c r="K11" s="6">
-        <v>12.65</v>
+        <v>12.4</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>17</v>
@@ -951,26 +944,26 @@
       <c r="D12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="9">
         <v>0.11799999999999999</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="10">
         <v>0.105</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="10">
         <v>9.64E-2</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="10">
         <v>9.8400000000000001E-2</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="10">
         <v>0.16200000000000001</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="11">
         <v>0.16</v>
       </c>
-      <c r="K12" s="13">
-        <v>0.155</v>
+      <c r="K12" s="10">
+        <v>0.152</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>17</v>
@@ -989,26 +982,26 @@
       <c r="D13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="9">
         <v>0.25900000000000001</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="10">
         <v>0.17699999999999999</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="10">
         <v>0.157</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="10">
         <v>0.182</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="10">
         <v>0.35599999999999998</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="11">
         <v>0.34399999999999997</v>
       </c>
-      <c r="K13" s="13">
-        <v>0.35</v>
+      <c r="K13" s="10">
+        <v>0.40400000000000003</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>17</v>
@@ -1027,26 +1020,26 @@
       <c r="D14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="9">
         <v>0.17499999999999999</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="10">
         <v>0.158</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="10">
         <v>0.14799999999999999</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="10">
         <v>0.184</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="10">
         <v>0.32900000000000001</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="11">
         <v>0.29799999999999999</v>
       </c>
-      <c r="K14" s="13">
-        <v>0.25</v>
+      <c r="K14" s="10">
+        <v>0.24299999999999999</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>17</v>
@@ -1065,26 +1058,26 @@
       <c r="D15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="9">
         <v>0.34599999999999997</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="10">
         <v>0.20899999999999999</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="10">
         <v>0.17799999999999999</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="10">
         <v>0.23300000000000001</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="10">
         <v>0.36499999999999999</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="11">
         <v>0.35599999999999998</v>
       </c>
-      <c r="K15" s="13">
-        <v>0.35</v>
+      <c r="K15" s="10">
+        <v>0.36899999999999999</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>17</v>
@@ -1103,26 +1096,26 @@
       <c r="D16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="9">
         <v>0.254</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="10">
         <v>0.215</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="10">
         <v>0.15</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="10">
         <v>0.20200000000000001</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="10">
         <v>0.33300000000000002</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="11">
         <v>0.32700000000000001</v>
       </c>
-      <c r="K16" s="13">
-        <v>0.33</v>
+      <c r="K16" s="10">
+        <v>0.35699999999999998</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>17</v>
@@ -1141,26 +1134,26 @@
       <c r="D17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="9">
         <v>0.17199999999999999</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="10">
         <v>0.17399999999999999</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="10">
         <v>0.19500000000000001</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="10">
         <v>0.21299999999999999</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="10">
         <v>0.32900000000000001</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="11">
         <v>0.27800000000000002</v>
       </c>
-      <c r="K17" s="13">
-        <v>0.19800000000000001</v>
+      <c r="K17" s="10">
+        <v>0.21199999999999999</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>17</v>
@@ -1179,26 +1172,26 @@
       <c r="D18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="9">
         <v>9.5299999999999994</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="10">
         <v>9.89</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="10">
         <v>9.15</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="10">
         <v>11.1</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="10">
         <v>25.9</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="11">
         <v>17.5</v>
       </c>
-      <c r="K18" s="6">
-        <v>12.8</v>
+      <c r="K18" s="10">
+        <v>12.1</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>17</v>
@@ -1217,26 +1210,26 @@
       <c r="D19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="9">
         <v>0.30199999999999999</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="10">
         <v>0.28599999999999998</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="10">
         <v>0.26600000000000001</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="10">
         <v>0.26700000000000002</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="10">
         <v>0.311</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="11">
         <v>0.42099999999999999</v>
       </c>
-      <c r="K19" s="13">
-        <v>0.28000000000000003</v>
+      <c r="K19" s="10">
+        <v>0.57899999999999996</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>17</v>
@@ -1255,26 +1248,26 @@
       <c r="D20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="9">
         <v>0.192</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="10">
         <v>0.185</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="10">
         <v>0.20200000000000001</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="10">
         <v>0.22600000000000001</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="10">
         <v>0.188</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="11">
         <v>0.216</v>
       </c>
-      <c r="K20" s="13">
-        <v>0.19</v>
+      <c r="K20" s="10">
+        <v>0.2</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>17</v>
@@ -1293,26 +1286,26 @@
       <c r="D21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="9">
         <v>0.186</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="10">
         <v>0.20300000000000001</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="10">
         <v>0.19900000000000001</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="10">
         <v>0.215</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="10">
         <v>0.255</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="11">
         <v>0.33300000000000002</v>
       </c>
-      <c r="K21" s="13">
-        <v>0.20499999999999999</v>
+      <c r="K21" s="10">
+        <v>0.36</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>17</v>
@@ -1331,26 +1324,26 @@
       <c r="D22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="9">
         <v>0.23</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="10">
         <v>0.222</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="10">
         <v>0.24199999999999999</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="10">
         <v>0.27100000000000002</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="10">
         <v>0.22600000000000001</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="11">
         <v>0.25900000000000001</v>
       </c>
-      <c r="K22" s="13">
-        <v>0.22800000000000001</v>
+      <c r="K22" s="10">
+        <v>0.24</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>17</v>
@@ -1369,26 +1362,26 @@
       <c r="D23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="9">
         <v>0.34</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="10">
         <v>0.35</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="10">
         <v>0.37</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="10">
         <v>0.37</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="10">
         <v>0.39</v>
       </c>
-      <c r="J23" s="14">
+      <c r="J23" s="11">
         <v>0.41</v>
       </c>
-      <c r="K23" s="13">
-        <v>0.41</v>
+      <c r="K23" s="10">
+        <v>0.4</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>17</v>
@@ -1407,26 +1400,26 @@
       <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="9">
         <v>0.3357</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="10">
         <v>0.3453</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="10">
         <v>0.30580000000000002</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="10">
         <v>0.33929999999999999</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="10">
         <v>0.46750000000000003</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="11">
         <v>0.45329999999999998</v>
       </c>
-      <c r="K24" s="13">
-        <v>0.3982</v>
+      <c r="K24" s="10">
+        <v>0.39489999999999997</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>17</v>
@@ -1445,26 +1438,26 @@
       <c r="D25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="9">
         <v>0.115</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="10">
         <v>0.108</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G25" s="10">
         <v>0.12</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="10">
         <v>0.126</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="10">
         <v>0.13600000000000001</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="11">
         <v>0.16700000000000001</v>
       </c>
-      <c r="K25" s="13">
-        <v>0.16</v>
+      <c r="K25" s="10">
+        <v>0.159</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>17</v>
@@ -1483,132 +1476,132 @@
       <c r="D26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="9">
         <v>0.11700000000000001</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="10">
         <v>0.123</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G26" s="10">
         <v>0.11600000000000001</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="10">
         <v>0.13100000000000001</v>
       </c>
-      <c r="I26" s="13">
+      <c r="I26" s="10">
         <v>0.13900000000000001</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="11">
         <v>0.182</v>
       </c>
-      <c r="K26" s="13">
-        <v>0.17499999999999999</v>
+      <c r="K26" s="10">
+        <v>0.17199999999999999</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="14">
         <v>0.20100000000000001</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="15">
         <v>0.21099999999999999</v>
       </c>
-      <c r="G27" s="18">
+      <c r="G27" s="15">
         <v>0.216</v>
       </c>
-      <c r="H27" s="18">
+      <c r="H27" s="15">
         <v>0.22600000000000001</v>
       </c>
-      <c r="I27" s="18">
+      <c r="I27" s="15">
         <v>0.31900000000000001</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J27" s="16">
         <v>0.40899999999999997</v>
       </c>
-      <c r="K27" s="18">
-        <v>0.3</v>
-      </c>
-      <c r="L27" s="20" t="s">
+      <c r="K27" s="15">
+        <v>0.223</v>
+      </c>
+      <c r="L27" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
     </row>
     <row r="30" spans="1:12" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
     </row>
     <row r="31" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
     </row>
     <row r="32" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>